<commit_message>
atualizando as sprints e adicionando o Burndownchart
</commit_message>
<xml_diff>
--- a/Docs/Sprints/Sprint II/Organização Sprints.xlsx
+++ b/Docs/Sprints/Sprint II/Organização Sprints.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.nascimento\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fazenda-Urbana\Docs\Sprints\Sprint II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183A5560-17AA-4836-BE7C-D4CA70D0D149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119105BE-EBE0-49A3-A788-30E032D88CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -787,7 +787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -821,94 +821,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -917,59 +935,26 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1254,25 +1239,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:I40"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26:I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="134.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="134.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="117.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="143.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="134.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="117.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1272,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1302,7 +1287,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1317,7 +1302,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1332,7 +1317,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1347,7 +1332,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1362,7 +1347,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1377,10 +1362,10 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>29</v>
@@ -1389,916 +1374,913 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="44" t="s">
+      <c r="K11" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="28"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="46"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="41"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="51"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="33"/>
-      <c r="G13" s="47" t="s">
+      <c r="C13" s="27"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="36"/>
+      <c r="G13" s="46" t="s">
         <v>81</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="48"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="43"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
       <c r="B14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="34"/>
-      <c r="G14" s="47"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="37"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="49"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="44"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="34"/>
-      <c r="G15" s="47"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="37"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="49"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="35"/>
-      <c r="G16" s="47"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="38"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="50"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="52"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="45"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="33"/>
-      <c r="G18" s="53" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="36"/>
+      <c r="G18" s="42" t="s">
         <v>82</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="48"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="43"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
       <c r="B19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="34"/>
-      <c r="G19" s="53"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="37"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="49"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="44"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="35"/>
-      <c r="G20" s="53"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="38"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="50"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="52"/>
-    </row>
-    <row r="22" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="45"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="33"/>
-      <c r="G22" s="47" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="36"/>
+      <c r="G22" s="46" t="s">
         <v>83</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="48"/>
-    </row>
-    <row r="23" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="43"/>
+    </row>
+    <row r="23" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
       <c r="B23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="34"/>
-      <c r="G23" s="47"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="37"/>
+      <c r="G23" s="46"/>
       <c r="H23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="49"/>
-    </row>
-    <row r="24" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="35"/>
-      <c r="G24" s="47"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="38"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="50"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="52"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="45"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="33"/>
-      <c r="G26" s="47" t="s">
+      <c r="C26" s="27"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="36"/>
+      <c r="G26" s="46" t="s">
         <v>84</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="59"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="48"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
+        <v>41</v>
+      </c>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="43"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
       <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="34"/>
-      <c r="G27" s="47"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="37"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="60"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="49"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="44"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="35"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="61"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="50"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="52"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
+      <c r="C28" s="29"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="38"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="45"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="33"/>
-      <c r="G30" s="47" t="s">
+      <c r="C30" s="27"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="36"/>
+      <c r="G30" s="46" t="s">
         <v>85</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" s="59"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="48"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="43"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
       <c r="B31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="34"/>
-      <c r="G31" s="47"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="37"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I31" s="60"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="49"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+        <v>32</v>
+      </c>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="44"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="35"/>
-      <c r="G32" s="47"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="38"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32" s="61"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="50"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="52"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="45"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="20"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="33"/>
-      <c r="G34" s="47" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="36"/>
+      <c r="G34" s="46" t="s">
         <v>86</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="48"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="43"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
       <c r="B35" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="34"/>
-      <c r="G35" s="47"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="37"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="49"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="44"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="35"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="50"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="52"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="38"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="45"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="16"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="20"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="33"/>
-      <c r="G38" s="53" t="s">
+      <c r="C38" s="27"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="36"/>
+      <c r="G38" s="42" t="s">
         <v>87</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38" s="59"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="48"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
+        <v>35</v>
+      </c>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="43"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
       <c r="B39" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="34"/>
-      <c r="G39" s="53"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="37"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I39" s="60"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="49"/>
-    </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="44"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="33"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="35"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56" t="s">
+      <c r="C40" s="29"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="38"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I40" s="62"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="58"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="54"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="33"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="36"/>
+      <c r="G42" s="55"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
       <c r="B43" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="34"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="37"/>
+      <c r="G43" s="55"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="56"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
       <c r="B44" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="35"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="29"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="37"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="38"/>
+      <c r="G44" s="55"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="33"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="36"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
       <c r="B47" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="34"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="K47" s="39"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="37"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
       <c r="B48" s="9"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="35"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="29"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="38"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="56"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="33"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="14"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="36"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
       <c r="B51" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="34"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="14"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="37"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
       <c r="B52" s="9"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="35"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="29"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="32"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="14" t="s">
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="38"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="16"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="23" t="s">
         <v>48</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="33"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="14"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="36"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="56"/>
+      <c r="J54" s="56"/>
+      <c r="K54" s="56"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
       <c r="B55" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="34"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="37"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="56"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
       <c r="B56" s="10"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="35"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="29"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="32"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="37"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="38"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="56"/>
+      <c r="J56" s="56"/>
+      <c r="K56" s="56"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="16"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
         <v>49</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="33"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="36"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="33"/>
       <c r="B59" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="34"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="37"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="56"/>
+      <c r="K59" s="56"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="33"/>
       <c r="B60" s="9"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="35"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="29"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="37"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="14" t="s">
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="38"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="56"/>
+      <c r="J60" s="56"/>
+      <c r="K60" s="56"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="16"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="33"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="14"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="36"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="56"/>
+      <c r="J62" s="56"/>
+      <c r="K62" s="56"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
       <c r="B63" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="34"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="14"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="37"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="56"/>
+      <c r="J63" s="56"/>
+      <c r="K63" s="56"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
       <c r="B64" s="9"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="35"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="29"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="37"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="37"/>
-    </row>
-    <row r="66" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="14" t="s">
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="38"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="56"/>
+      <c r="J64" s="56"/>
+      <c r="K64" s="56"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="16"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+    </row>
+    <row r="66" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="33"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="36"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-    </row>
-    <row r="67" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="36"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="56"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="56"/>
+    </row>
+    <row r="67" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
       <c r="B67" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="34"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-    </row>
-    <row r="68" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="37"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="56"/>
+      <c r="J67" s="56"/>
+      <c r="K67" s="56"/>
+    </row>
+    <row r="68" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
       <c r="B68" s="9"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="35"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="29"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="32"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="37"/>
-      <c r="I69" s="37"/>
-      <c r="J69" s="37"/>
-      <c r="K69" s="37"/>
-    </row>
-    <row r="70" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="14" t="s">
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="38"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="56"/>
+      <c r="J68" s="56"/>
+      <c r="K68" s="56"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="16"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="33"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="39"/>
-    </row>
-    <row r="71" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="36"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="56"/>
+      <c r="J70" s="56"/>
+      <c r="K70" s="56"/>
+    </row>
+    <row r="71" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="23"/>
       <c r="B71" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="34"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="39"/>
-      <c r="K71" s="39"/>
-    </row>
-    <row r="72" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="15"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="37"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="56"/>
+      <c r="J71" s="56"/>
+      <c r="K71" s="56"/>
+    </row>
+    <row r="72" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="24"/>
       <c r="B72" s="12"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="35"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="39"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C72" s="39"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="38"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="56"/>
+      <c r="J72" s="56"/>
+      <c r="K72" s="56"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
     </row>
   </sheetData>
@@ -2368,10 +2350,6 @@
     <mergeCell ref="I13:I16"/>
     <mergeCell ref="J13:J16"/>
     <mergeCell ref="K13:K16"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="E62:E64"/>
     <mergeCell ref="E66:E68"/>
     <mergeCell ref="E70:E72"/>
     <mergeCell ref="D66:D68"/>
@@ -2390,7 +2368,6 @@
     <mergeCell ref="D54:D56"/>
     <mergeCell ref="D58:D60"/>
     <mergeCell ref="D62:D64"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="E13:E16"/>
     <mergeCell ref="D18:D20"/>
@@ -2411,6 +2388,10 @@
     <mergeCell ref="C50:C52"/>
     <mergeCell ref="C54:C56"/>
     <mergeCell ref="C58:C60"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="E62:E64"/>
     <mergeCell ref="A62:A64"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="A70:A72"/>
@@ -2433,6 +2414,7 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Adicionando o dicionario de dados
</commit_message>
<xml_diff>
--- a/Docs/Sprints/Sprint II/Organização Sprints.xlsx
+++ b/Docs/Sprints/Sprint II/Organização Sprints.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Luiz\Desktop\Fazenda-Urbana\Docs\Sprints\Sprint II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francisco.monteiro\Desktop\Fazenda-Urbana\Docs\Sprints\Sprint II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D60B3A-0F71-440C-8493-054E06BF012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C85D903-0450-41D3-90E3-5F80E6144B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -355,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,18 +397,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -794,7 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -846,6 +845,140 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -858,158 +991,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1294,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35:H41"/>
+    <sheetView tabSelected="1" topLeftCell="G18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,108 +1420,108 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="63" t="s">
+      <c r="G11" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="49" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="37"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="67"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="61"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="50"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="65" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="32"/>
-      <c r="G13" s="56" t="s">
+      <c r="C13" s="62"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="51"/>
+      <c r="G13" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="60" t="s">
+      <c r="H13" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="68"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="33"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="68"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="52"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="33"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="68"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="52"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="34"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="68"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="53"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="37"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
@@ -1546,57 +1529,57 @@
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
-      <c r="G17" s="69"/>
+      <c r="G17" s="26"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="69" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="32"/>
-      <c r="G18" s="41" t="s">
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="51"/>
+      <c r="G18" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="62" t="s">
+      <c r="H18" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="68"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="37"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="33"/>
-      <c r="G19" s="41"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="52"/>
+      <c r="G19" s="44"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="68"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="34"/>
-      <c r="G20" s="41"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="53"/>
+      <c r="G20" s="44"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="68"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -1604,61 +1587,61 @@
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
-      <c r="G21" s="70"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="65" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="32"/>
-      <c r="G22" s="56" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="51"/>
+      <c r="G22" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="68"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="37"/>
     </row>
     <row r="23" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="33"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="62" t="s">
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="52"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="68"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="37"/>
     </row>
     <row r="24" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="34"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="62" t="s">
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="53"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="68"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
@@ -1666,59 +1649,59 @@
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
-      <c r="G25" s="70"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="16"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="32"/>
-      <c r="G26" s="56" t="s">
+      <c r="C26" s="62"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="51"/>
+      <c r="G26" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="62" t="s">
+      <c r="H26" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="68"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="37"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="33"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="62" t="s">
+      <c r="C27" s="63"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="52"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="68"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="37"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="34"/>
-      <c r="G28" s="56"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="53"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="68"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="37"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
@@ -1726,73 +1709,73 @@
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
-      <c r="G29" s="70"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="16"/>
     </row>
     <row r="30" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="65" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="32"/>
-      <c r="G30" s="56" t="s">
+      <c r="C30" s="62"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="51"/>
+      <c r="G30" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="H30" s="62" t="s">
+      <c r="H30" s="24" t="s">
         <v>47</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="71"/>
+      <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="33"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="50" t="s">
+      <c r="C31" s="63"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="52"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="23" t="s">
         <v>89</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="71"/>
+      <c r="K31" s="25"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="33"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="62" t="s">
+      <c r="C32" s="63"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="52"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="24" t="s">
         <v>43</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="71"/>
+      <c r="K32" s="25"/>
     </row>
     <row r="33" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="65"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="33"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="62" t="s">
+      <c r="C33" s="63"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="52"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="24" t="s">
         <v>38</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="72"/>
+      <c r="K33" s="28"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
@@ -1800,63 +1783,63 @@
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="16"/>
-      <c r="G34" s="70"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="16"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="65" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="32"/>
-      <c r="G35" s="48" t="s">
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="51"/>
+      <c r="G35" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="73"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="28"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="33"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="47" t="s">
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="52"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="73"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="28"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="65"/>
       <c r="B37" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="34"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="47" t="s">
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="53"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="73"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="28"/>
     </row>
     <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
@@ -1864,69 +1847,67 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="16"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="47" t="s">
+      <c r="G38" s="39"/>
+      <c r="H38" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="73"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="28"/>
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="69" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="32"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="49" t="s">
+      <c r="C39" s="62"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="51"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="73"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="28"/>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="33"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="50" t="s">
+      <c r="C40" s="63"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="52"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="73"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="28"/>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="69"/>
       <c r="B41" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="33"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="57" t="s">
+      <c r="C41" s="63"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="52"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="54"/>
+      <c r="K41" s="21"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
+      <c r="A42" s="69"/>
       <c r="B42" s="9"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="34"/>
-      <c r="G42" s="70"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="53"/>
+      <c r="G42" s="27"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -1938,59 +1919,56 @@
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
       <c r="E43" s="16"/>
-      <c r="G43" s="43" t="s">
+      <c r="G43" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="53" t="s">
+      <c r="H43" t="s">
         <v>92</v>
       </c>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="74"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="29"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="65" t="s">
         <v>52</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="32"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="74"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="51"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="29"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="33"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="75"/>
-      <c r="I45" s="75"/>
-      <c r="J45" s="75"/>
-      <c r="K45" s="76"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="52"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="31"/>
     </row>
     <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="34"/>
-      <c r="G46" s="42"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="53"/>
+      <c r="G46" s="19"/>
       <c r="H46" s="17"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
@@ -2000,49 +1978,49 @@
       <c r="E47" s="16"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="65" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="32"/>
-      <c r="G48" s="38"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="51"/>
+      <c r="G48" s="32"/>
       <c r="H48" s="17"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="33"/>
-      <c r="G49" s="38"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="52"/>
+      <c r="G49" s="32"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="9"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="34"/>
-      <c r="G50" s="38"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="53"/>
+      <c r="G50" s="32"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
@@ -2056,43 +2034,43 @@
       <c r="K51" s="1"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="65" t="s">
         <v>46</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="32"/>
-      <c r="G52" s="38"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="51"/>
+      <c r="G52" s="32"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="33"/>
-      <c r="G53" s="38"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="52"/>
+      <c r="G53" s="32"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="34"/>
-      <c r="G54" s="38"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="53"/>
+      <c r="G54" s="32"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
@@ -2107,46 +2085,46 @@
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="65" t="s">
         <v>47</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="32"/>
-      <c r="G56" s="38"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="51"/>
+      <c r="G56" s="32"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="33"/>
-      <c r="G57" s="38"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="52"/>
+      <c r="G57" s="32"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="10"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="34"/>
-      <c r="G58" s="38"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="53"/>
+      <c r="G58" s="32"/>
       <c r="H58" s="17"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
@@ -2161,46 +2139,46 @@
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="69" t="s">
         <v>48</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="32"/>
-      <c r="G60" s="40"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="51"/>
+      <c r="G60" s="34"/>
       <c r="H60" s="17"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="69"/>
       <c r="B61" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="33"/>
-      <c r="G61" s="40"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="52"/>
+      <c r="G61" s="34"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
+      <c r="A62" s="69"/>
       <c r="B62" s="9"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="34"/>
-      <c r="G62" s="40"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="53"/>
+      <c r="G62" s="34"/>
       <c r="H62" s="17"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="33"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
@@ -2215,46 +2193,46 @@
       <c r="K63" s="1"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="65" t="s">
         <v>49</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="32"/>
-      <c r="G64" s="38"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="51"/>
+      <c r="G64" s="32"/>
       <c r="H64" s="17"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
+      <c r="A65" s="65"/>
       <c r="B65" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="33"/>
-      <c r="G65" s="38"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="52"/>
+      <c r="G65" s="32"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="19"/>
+      <c r="A66" s="65"/>
       <c r="B66" s="9"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="34"/>
-      <c r="G66" s="38"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="53"/>
+      <c r="G66" s="32"/>
       <c r="H66" s="17"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
@@ -2269,46 +2247,46 @@
       <c r="K67" s="1"/>
     </row>
     <row r="68" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="65" t="s">
         <v>50</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="32"/>
-      <c r="G68" s="38"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="51"/>
+      <c r="G68" s="32"/>
       <c r="H68" s="17"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
     </row>
     <row r="69" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
+      <c r="A69" s="65"/>
       <c r="B69" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="33"/>
-      <c r="G69" s="38"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="52"/>
+      <c r="G69" s="32"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="39"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="33"/>
+      <c r="K69" s="33"/>
     </row>
     <row r="70" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
+      <c r="A70" s="65"/>
       <c r="B70" s="9"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="34"/>
-      <c r="G70" s="38"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="53"/>
+      <c r="G70" s="32"/>
       <c r="H70" s="17"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="39"/>
+      <c r="I70" s="33"/>
+      <c r="J70" s="33"/>
+      <c r="K70" s="33"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
@@ -2323,120 +2301,73 @@
       <c r="K71" s="1"/>
     </row>
     <row r="72" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="65" t="s">
         <v>51</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="32"/>
-      <c r="G72" s="38"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="51"/>
+      <c r="G72" s="32"/>
       <c r="H72" s="17"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="39"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33"/>
+      <c r="K72" s="33"/>
     </row>
     <row r="73" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="19"/>
+      <c r="A73" s="65"/>
       <c r="B73" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="33"/>
-      <c r="G73" s="38"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="39"/>
-      <c r="K73" s="39"/>
+      <c r="C73" s="55"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="52"/>
+      <c r="G73" s="32"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="33"/>
     </row>
     <row r="74" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="20"/>
+      <c r="A74" s="66"/>
       <c r="B74" s="12"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="28"/>
-      <c r="E74" s="34"/>
-      <c r="G74" s="38"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="39"/>
-      <c r="K74" s="39"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="53"/>
+      <c r="G74" s="32"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="33"/>
+      <c r="K74" s="33"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="J68:J70"/>
-    <mergeCell ref="K68:K70"/>
-    <mergeCell ref="G72:G74"/>
-    <mergeCell ref="I72:I74"/>
-    <mergeCell ref="J72:J74"/>
-    <mergeCell ref="K72:K74"/>
-    <mergeCell ref="G60:G62"/>
-    <mergeCell ref="I60:I62"/>
-    <mergeCell ref="J60:J62"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="G64:G66"/>
-    <mergeCell ref="I64:I66"/>
-    <mergeCell ref="J64:J66"/>
-    <mergeCell ref="K64:K66"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="J52:J54"/>
-    <mergeCell ref="K52:K54"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="I56:I58"/>
-    <mergeCell ref="J56:J58"/>
-    <mergeCell ref="K56:K58"/>
-    <mergeCell ref="G48:G50"/>
-    <mergeCell ref="I48:I50"/>
-    <mergeCell ref="J48:J50"/>
-    <mergeCell ref="K48:K50"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="K26:K28"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="G35:G41"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="I13:I16"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="K13:K16"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="E72:E74"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="D72:D74"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="E13:E16"/>
     <mergeCell ref="D18:D20"/>
@@ -2461,29 +2392,76 @@
     <mergeCell ref="E56:E58"/>
     <mergeCell ref="E60:E62"/>
     <mergeCell ref="E64:E66"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="K13:K16"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="K26:K28"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="G35:G41"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="J52:J54"/>
+    <mergeCell ref="K52:K54"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="I56:I58"/>
+    <mergeCell ref="J56:J58"/>
+    <mergeCell ref="K56:K58"/>
+    <mergeCell ref="G48:G50"/>
+    <mergeCell ref="I48:I50"/>
+    <mergeCell ref="J48:J50"/>
+    <mergeCell ref="K48:K50"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="J68:J70"/>
+    <mergeCell ref="K68:K70"/>
+    <mergeCell ref="G72:G74"/>
+    <mergeCell ref="I72:I74"/>
+    <mergeCell ref="J72:J74"/>
+    <mergeCell ref="K72:K74"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="I60:I62"/>
+    <mergeCell ref="J60:J62"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="G64:G66"/>
+    <mergeCell ref="I64:I66"/>
+    <mergeCell ref="J64:J66"/>
+    <mergeCell ref="K64:K66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>